<commit_message>
Add newsletter entry for May 2025: "Via con Dios, My Darlin" reflecting on a trip to Mexico
</commit_message>
<xml_diff>
--- a/0-admin/mia/2025-mia-harlock-time-tracker.xlsx
+++ b/0-admin/mia/2025-mia-harlock-time-tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28822"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28824"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/2025-theo/people/mia-cotton-harlock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="200" documentId="8_{E6B1AFC3-31B1-434E-8DFB-53589C29742B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A74193F6-2F22-4E28-82E6-A635D77D69B1}"/>
+  <xr:revisionPtr revIDLastSave="206" documentId="8_{E6B1AFC3-31B1-434E-8DFB-53589C29742B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E811D7C3-2C15-4371-8551-169C3F01AB80}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>Call &amp; Email to Doris about May health topic</t>
+  </si>
+  <si>
+    <t>Calls with Doris &amp; Theo / Health Topic Article: Our Parents, Our Self v1</t>
   </si>
 </sst>
 </file>
@@ -1578,7 +1581,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.45"/>
@@ -1636,11 +1639,19 @@
       </c>
       <c r="E3" s="23"/>
     </row>
-    <row r="4" spans="1:5" ht="18">
-      <c r="A4" s="31"/>
-      <c r="B4" s="30"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="23"/>
+    <row r="4" spans="1:5" ht="36">
+      <c r="A4" s="31">
+        <v>45775</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="39">
+        <v>3</v>
+      </c>
+      <c r="D4" s="23">
+        <v>150</v>
+      </c>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:5" ht="18">
@@ -1692,7 +1703,7 @@
       <c r="C11" s="38"/>
       <c r="D11" s="23">
         <f>SUM(D2:D10)</f>
-        <v>50</v>
+        <v>200</v>
       </c>
       <c r="E11" s="23">
         <f>SUM(E2:E10)</f>
@@ -1720,7 +1731,7 @@
       <c r="D14" s="23"/>
       <c r="E14" s="25">
         <f>D11-E11</f>
-        <v>50</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 2025-mia-harlock-time-tracker.xlsx with new data
</commit_message>
<xml_diff>
--- a/0-admin/mia/2025-mia-harlock-time-tracker.xlsx
+++ b/0-admin/mia/2025-mia-harlock-time-tracker.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28914"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/2025-theo/people/mia-cotton-harlock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="206" documentId="8_{E6B1AFC3-31B1-434E-8DFB-53589C29742B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E811D7C3-2C15-4371-8551-169C3F01AB80}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="8_{E6B1AFC3-31B1-434E-8DFB-53589C29742B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3408827C-3299-494D-B865-2430FEE95323}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="12" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>Calls with Doris &amp; Theo / Health Topic Article: Our Parents, Our Self v1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comms with Theo .5 / Email to residents re: hobbies .5 </t>
   </si>
 </sst>
 </file>
@@ -1580,7 +1583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D641B581-E755-456D-B6F9-40A5F9BD4A43}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
@@ -1743,8 +1746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C28470-7CA3-4651-BD84-53FB2703137D}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1771,10 +1774,16 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="17.45">
-      <c r="A2" s="12"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="7"/>
+    <row r="2" spans="1:5" ht="36">
+      <c r="A2" s="12">
+        <v>45797</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
@@ -1840,7 +1849,7 @@
       <c r="B11" s="4"/>
       <c r="C11" s="7">
         <f>SUM(C2:C10)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="6">
         <f>SUM(D2:D10)</f>

</xml_diff>

<commit_message>
Add HTML and Markdown files for "Theo Grief Tech" documentation
</commit_message>
<xml_diff>
--- a/0-admin/mia/2025-mia-harlock-time-tracker.xlsx
+++ b/0-admin/mia/2025-mia-harlock-time-tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/2025-theo/people/mia-cotton-harlock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="209" documentId="8_{E6B1AFC3-31B1-434E-8DFB-53589C29742B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3408827C-3299-494D-B865-2430FEE95323}"/>
+  <xr:revisionPtr revIDLastSave="214" documentId="8_{E6B1AFC3-31B1-434E-8DFB-53589C29742B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3DE7F1D-C211-4DD5-AF71-0EE2975B9DE4}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="January" sheetId="12" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t xml:space="preserve">Comms with Theo .5 / Email to residents re: hobbies .5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hobby article with link to study </t>
   </si>
 </sst>
 </file>
@@ -1747,7 +1750,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1787,14 +1790,20 @@
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:5" ht="17.45">
-      <c r="A3" s="13"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5"/>
+    <row r="3" spans="1:5" ht="18">
+      <c r="A3" s="13">
+        <v>45798</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:5" ht="17.45">
+    <row r="4" spans="1:5" ht="18">
       <c r="A4" s="13"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
@@ -1849,7 +1858,7 @@
       <c r="B11" s="4"/>
       <c r="C11" s="7">
         <f>SUM(C2:C10)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="6">
         <f>SUM(D2:D10)</f>

</xml_diff>

<commit_message>
Update health agenda with latest appointments and agenda items
</commit_message>
<xml_diff>
--- a/0-admin/mia/2025-mia-harlock-time-tracker.xlsx
+++ b/0-admin/mia/2025-mia-harlock-time-tracker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28922"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/2025-theo/people/mia-cotton-harlock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="214" documentId="8_{E6B1AFC3-31B1-434E-8DFB-53589C29742B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3DE7F1D-C211-4DD5-AF71-0EE2975B9DE4}"/>
+  <xr:revisionPtr revIDLastSave="219" documentId="8_{E6B1AFC3-31B1-434E-8DFB-53589C29742B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2809292-D363-4FA0-8520-A535B17BE2DB}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t xml:space="preserve">Hobby article with link to study </t>
+  </si>
+  <si>
+    <t>Record &amp; transcribe Jane's story / Toronto &gt; SF</t>
   </si>
 </sst>
 </file>
@@ -1750,7 +1753,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1804,14 +1807,22 @@
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" ht="18">
-      <c r="A4" s="13"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
+      <c r="A4" s="13">
+        <v>45801</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="17.45">
-      <c r="A5" s="13"/>
+    <row r="5" spans="1:5" ht="18">
+      <c r="A5" s="13">
+        <v>45804</v>
+      </c>
       <c r="B5" s="4"/>
       <c r="C5" s="5"/>
       <c r="D5" s="6"/>
@@ -1858,7 +1869,7 @@
       <c r="B11" s="4"/>
       <c r="C11" s="7">
         <f>SUM(C2:C10)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="6">
         <f>SUM(D2:D10)</f>

</xml_diff>

<commit_message>
Add Drew's M&A Prospect Checklist and introduce Karen McNeill to digital legacy concept
- Created a comprehensive checklist for evaluating small to medium-sized business prospects in mergers and acquisitions, ensuring it is actionable and easy to understand.
- Drafted an introductory message for Karen McNeill, highlighting a potential collaboration with Dan Thomson on digital legacy projects.
</commit_message>
<xml_diff>
--- a/0-admin/mia/2025-mia-harlock-time-tracker.xlsx
+++ b/0-admin/mia/2025-mia-harlock-time-tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4348e1419f457eb2/2025-theo/people/mia-cotton-harlock/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="219" documentId="8_{E6B1AFC3-31B1-434E-8DFB-53589C29742B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E2809292-D363-4FA0-8520-A535B17BE2DB}"/>
+  <xr:revisionPtr revIDLastSave="229" documentId="8_{E6B1AFC3-31B1-434E-8DFB-53589C29742B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0A32100C-DF67-4950-9EA8-2B9961C4878E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Record &amp; transcribe Jane's story / Toronto &gt; SF</t>
+  </si>
+  <si>
+    <t>Decoding transcription, editing Jane's story, sending out</t>
   </si>
 </sst>
 </file>
@@ -1753,7 +1756,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1790,7 +1793,9 @@
       <c r="C2" s="7">
         <v>1</v>
       </c>
-      <c r="D2" s="6"/>
+      <c r="D2" s="6">
+        <v>50</v>
+      </c>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="18">
@@ -1803,7 +1808,9 @@
       <c r="C3" s="5">
         <v>1</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="6">
+        <v>50</v>
+      </c>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" ht="18">
@@ -1816,16 +1823,24 @@
       <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="6">
+        <v>50</v>
+      </c>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:5" ht="18">
+    <row r="5" spans="1:5" ht="36">
       <c r="A5" s="13">
         <v>45804</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
+      <c r="B5" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="5">
+        <v>3</v>
+      </c>
+      <c r="D5" s="6">
+        <v>150</v>
+      </c>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" ht="17.45">
@@ -1869,11 +1884,11 @@
       <c r="B11" s="4"/>
       <c r="C11" s="7">
         <f>SUM(C2:C10)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D11" s="6">
         <f>SUM(D2:D10)</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="E11" s="6">
         <f>SUM(E2:E10)</f>
@@ -1901,7 +1916,7 @@
       <c r="D14" s="6"/>
       <c r="E14" s="10">
         <f>D11-E11</f>
-        <v>0</v>
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>